<commit_message>
beginnings of the excel file
</commit_message>
<xml_diff>
--- a/SRM Sizing/Output.xlsx
+++ b/SRM Sizing/Output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/81be7871ac33ab77/Documents/GitHub/purdue-orbital-mission-design/SRM Sizing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="140" documentId="8_{C7C79824-C540-4E01-B25D-0EC6B092111C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F8C45548-8FC9-4786-8D96-EF015B399113}"/>
+  <xr:revisionPtr revIDLastSave="141" documentId="8_{C7C79824-C540-4E01-B25D-0EC6B092111C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0DAECF83-284C-4353-BC75-7CD9F07519AF}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{9A591022-FAC3-46EB-B550-F4F5303FF3BC}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="14400" windowHeight="7350" xr2:uid="{9A591022-FAC3-46EB-B550-F4F5303FF3BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -244,6 +244,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -257,9 +260,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4608,7 +4608,7 @@
   <dimension ref="A1:S12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U12" sqref="U12"/>
+      <selection activeCell="D2" sqref="D2:D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -4617,28 +4617,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.75">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="12"/>
-      <c r="F1" s="13" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="13"/>
+      <c r="F1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.75">
       <c r="A2" s="6" t="s">
@@ -4657,7 +4657,7 @@
       <c r="B3" s="7"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.75">
@@ -4667,7 +4667,7 @@
       <c r="B4" s="7"/>
       <c r="C4" s="2"/>
       <c r="D4" s="3">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.75">
@@ -4677,7 +4677,7 @@
       <c r="B5" s="7"/>
       <c r="C5" s="2"/>
       <c r="D5" s="3">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.75">
@@ -4687,7 +4687,7 @@
       <c r="B6" s="7"/>
       <c r="C6" s="2"/>
       <c r="D6" s="3">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.75">
@@ -4697,7 +4697,7 @@
       <c r="B7" s="7"/>
       <c r="C7" s="2"/>
       <c r="D7" s="3">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.75">
@@ -4707,7 +4707,7 @@
       <c r="B8" s="7"/>
       <c r="C8" s="2"/>
       <c r="D8" s="3">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.75">
@@ -4717,7 +4717,7 @@
       <c r="B9" s="7"/>
       <c r="C9" s="2"/>
       <c r="D9" s="3">
-        <v>15</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.75">
@@ -4727,7 +4727,7 @@
       <c r="B10" s="7"/>
       <c r="C10" s="2"/>
       <c r="D10" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.75">
@@ -4737,26 +4737,21 @@
       <c r="B11" s="7"/>
       <c r="C11" s="2"/>
       <c r="D11" s="3">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="15.5" thickBot="1" x14ac:dyDescent="0.9">
-      <c r="A12" s="8" t="s">
+      <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="9"/>
+      <c r="B12" s="10"/>
       <c r="C12" s="4"/>
       <c r="D12" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="F1:S1"/>
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A1:D1"/>
@@ -4765,6 +4760,11 @@
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="F1:S1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
@@ -4792,22 +4792,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.75">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="D1" s="13" t="s">
+      <c r="B1" s="8"/>
+      <c r="D1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="13"/>
-      <c r="G1" s="13" t="s">
+      <c r="E1" s="8"/>
+      <c r="G1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="13"/>
-      <c r="J1" s="13" t="s">
+      <c r="H1" s="8"/>
+      <c r="J1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="13"/>
+      <c r="K1" s="8"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.75">
       <c r="A2" s="1" t="s">

</xml_diff>